<commit_message>
Author           : Shubham Jain Story Id         : 49, 52 Files Modified   : ShubhamJain.xlsx Description      : Sprint Tracking Sheet modified for listing tasks breakdown
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/ShubhamJain.xlsx
+++ b/TeamDetails/TasksBreakDown/ShubhamJain.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham Jain\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSDMS Project\Project\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Task ID</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Display FAQ Question using basic HTML</t>
-  </si>
-  <si>
-    <t>Designing of the FAQ page should be done by Angular UI Bootstrap</t>
   </si>
   <si>
     <t>T1</t>
@@ -138,9 +135,6 @@
     <t>T13</t>
   </si>
   <si>
-    <t>Creating a block diagram of FAQ</t>
-  </si>
-  <si>
     <t>T14</t>
   </si>
   <si>
@@ -148,6 +142,42 @@
   </si>
   <si>
     <t xml:space="preserve">                                                             UI Grid</t>
+  </si>
+  <si>
+    <t>Create a block diagram of FAQ</t>
+  </si>
+  <si>
+    <t>Design of the FAQ page should be done by Angular UI Bootstrap</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>Unit testing</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>Code Review &amp; Feedback</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>Incorporate Feedback</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>Maintainance</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>SVN Commit</t>
   </si>
 </sst>
 </file>
@@ -233,7 +263,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -246,19 +276,25 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -570,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,138 +622,155 @@
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="9">
+        <f>SUM(F2:F20)</f>
+        <v>41</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4">
+        <f>F2-G2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4">
         <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="7">
-        <f>SUM(F3:F16)</f>
-        <v>39</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="4">
-        <v>2</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4">
-        <f>F3-G3</f>
+        <f t="shared" ref="H3:H20" si="0">F3-G3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4">
         <v>1</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4">
-        <f t="shared" ref="H4:H16" si="0">F4-G4</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="4">
-        <v>2</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>29</v>
+      <c r="E8" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
@@ -729,90 +782,90 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>36</v>
+      <c r="E9" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="F9" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>37</v>
+      <c r="C10" s="9"/>
+      <c r="D10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="F10" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>34</v>
+      <c r="C11" s="9"/>
+      <c r="D11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="F11" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>7</v>
+      <c r="E12" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="F12" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>18</v>
+      <c r="E13" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="F13" s="4">
         <v>3</v>
@@ -824,91 +877,135 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>22</v>
+      <c r="E15" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="F15" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>8</v>
+      <c r="C16" s="9"/>
+      <c r="D16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="F16" s="4">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E17"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
@@ -1166,7 +1263,7 @@
   <mergeCells count="3">
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B3:B16"/>
-    <mergeCell ref="C3:C16"/>
+    <mergeCell ref="C2:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author           : Shubham Jain Story Id         : 49, 52 Files Modified   : ShubhamJain.xlsx Description      : Sprint Tracking Sheet modified,reviewed by Ruchi Pareek.
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/ShubhamJain.xlsx
+++ b/TeamDetails/TasksBreakDown/ShubhamJain.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSDMS Project\Project\trunk\TeamDetails\TasksBreakDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2017\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Task ID</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Story Estimate</t>
-  </si>
-  <si>
-    <t>Basic Structure of FAQ Page</t>
   </si>
   <si>
     <t>Display FAQ Question using basic HTML</t>
@@ -162,29 +159,14 @@
     <t>Code Review &amp; Feedback</t>
   </si>
   <si>
-    <t>T17</t>
-  </si>
-  <si>
-    <t>Incorporate Feedback</t>
-  </si>
-  <si>
-    <t>T18</t>
-  </si>
-  <si>
-    <t>Maintainance</t>
-  </si>
-  <si>
-    <t>T19</t>
-  </si>
-  <si>
-    <t>SVN Commit</t>
+    <t>Create Structure of FAQ Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +185,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -229,12 +218,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -257,13 +246,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -281,25 +307,31 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
-    <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
+    <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -608,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,6 +655,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
@@ -643,21 +681,21 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="10">
         <f>SUM(F2:F20)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="F2" s="4">
         <v>2</v>
@@ -669,51 +707,47 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H20" si="0">F3-G3</f>
+        <f t="shared" ref="H3:H17" si="0">F3-G3</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -725,14 +759,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -744,14 +778,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="4">
         <v>4</v>
@@ -763,14 +797,14 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
@@ -782,14 +816,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="4">
         <v>3</v>
@@ -801,14 +835,14 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -820,14 +854,14 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>7</v>
+        <v>28</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="F11" s="4">
         <v>4</v>
@@ -839,14 +873,14 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="4">
         <v>3</v>
@@ -858,14 +892,14 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4">
         <v>3</v>
@@ -877,14 +911,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="4">
         <v>6</v>
@@ -896,14 +930,14 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="F15" s="4">
         <v>4</v>
@@ -915,14 +949,14 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="11"/>
       <c r="D16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="F16" s="4">
         <v>0.5</v>
@@ -934,17 +968,19 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="9"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>0.5</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
@@ -953,59 +989,17 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="4">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
+      <c r="E18"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="11">
-        <v>1</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="E19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="4">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
+      <c r="E20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
@@ -1261,9 +1255,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B3:B16"/>
-    <mergeCell ref="C2:C20"/>
+    <mergeCell ref="C2:C17"/>
+    <mergeCell ref="B2:B17"/>
+    <mergeCell ref="A2:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author           : Shubham Jain Story Id         : 49, 52 Files Modified   : ShubhamJain.xlsx Description      : Sprint Tracking Sheet modified
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/ShubhamJain.xlsx
+++ b/TeamDetails/TasksBreakDown/ShubhamJain.xlsx
@@ -166,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,8 +196,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +230,13 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -283,13 +296,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -313,9 +342,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -325,14 +351,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -640,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,10 +715,10 @@
       <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <f>SUM(F2:F20)</f>
         <v>39</v>
       </c>
@@ -700,16 +731,18 @@
       <c r="F2" s="4">
         <v>2</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4">
+        <v>2</v>
+      </c>
       <c r="H2" s="4">
         <f>F2-G2</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
@@ -719,16 +752,18 @@
       <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H17" si="0">F3-G3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
@@ -741,8 +776,8 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
@@ -752,16 +787,18 @@
       <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
@@ -771,16 +808,18 @@
       <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
@@ -790,16 +829,18 @@
       <c r="F7" s="4">
         <v>4</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
@@ -817,8 +858,8 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
@@ -836,8 +877,8 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="6" t="s">
         <v>21</v>
       </c>
@@ -847,16 +888,18 @@
       <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
       <c r="H10" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="6" t="s">
         <v>28</v>
       </c>
@@ -874,8 +917,8 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="6" t="s">
         <v>29</v>
       </c>
@@ -893,8 +936,8 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="6" t="s">
         <v>30</v>
       </c>
@@ -912,8 +955,8 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="6" t="s">
         <v>31</v>
       </c>
@@ -931,8 +974,8 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="6" t="s">
         <v>32</v>
       </c>
@@ -950,8 +993,8 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="6" t="s">
         <v>37</v>
       </c>
@@ -969,8 +1012,8 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="6" t="s">
         <v>39</v>
       </c>
@@ -990,6 +1033,10 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="E18"/>
+      <c r="H18" s="14">
+        <f>SUM(H2:H17)</f>
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>

</xml_diff>

<commit_message>
Author                       :Shubham Jain Task                         :Track the hour burnt to implement the story assigned in Sprint-2 File Modified                :ShubhamJain.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/ShubhamJain.xlsx
+++ b/TeamDetails/TasksBreakDown/ShubhamJain.xlsx
@@ -342,6 +342,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -357,7 +358,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,13 +712,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="10">
         <f>SUM(F2:F20)</f>
         <v>39</v>
       </c>
@@ -740,9 +740,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="10"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
@@ -761,9 +761,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="10"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
@@ -775,9 +775,9 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
@@ -788,17 +788,17 @@
         <v>2</v>
       </c>
       <c r="G5" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
@@ -817,9 +817,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
@@ -830,17 +830,17 @@
         <v>4</v>
       </c>
       <c r="G7" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
@@ -850,16 +850,18 @@
       <c r="F8" s="4">
         <v>4</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4">
+        <v>2</v>
+      </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="10"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
@@ -869,16 +871,18 @@
       <c r="F9" s="4">
         <v>3</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
       <c r="H9" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="6" t="s">
         <v>21</v>
       </c>
@@ -897,9 +901,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="6" t="s">
         <v>28</v>
       </c>
@@ -916,9 +920,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="6" t="s">
         <v>29</v>
       </c>
@@ -935,9 +939,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="6" t="s">
         <v>30</v>
       </c>
@@ -954,9 +958,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="6" t="s">
         <v>31</v>
       </c>
@@ -973,9 +977,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="6" t="s">
         <v>32</v>
       </c>
@@ -992,9 +996,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="10"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="11"/>
       <c r="D16" s="6" t="s">
         <v>37</v>
       </c>
@@ -1011,9 +1015,9 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="11"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="6" t="s">
         <v>39</v>
       </c>
@@ -1033,9 +1037,9 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="E18"/>
-      <c r="H18" s="14">
+      <c r="H18" s="9">
         <f>SUM(H2:H17)</f>
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>